<commit_message>
fix: not empty input on name entry
</commit_message>
<xml_diff>
--- a/profiles.xlsx
+++ b/profiles.xlsx
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +425,77 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>description</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>3</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Aluno</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Ambiente virtual para o aluno estudar.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>4</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Professor</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Verificar a nota dos Alunos</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Diretor</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Verificar eficiências dos professores.</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>